<commit_message>
First time commit from work computer
</commit_message>
<xml_diff>
--- a/ArendseeExperiment/20220800SequentalExtractions.xlsx
+++ b/ArendseeExperiment/20220800SequentalExtractions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuppevelt\Nextcloud\Documents\DATA\Arendsee_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Nextcloud\Documents\DATA\Code\PhD_thesis\ArendseeExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD92F66-2B30-4925-A5BE-9BE051F08D1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB3B10E-7663-4CFA-8172-A60343E8E058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6AC47CB-9B1F-48AB-B77D-F5FF670D77EC}"/>
   </bookViews>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD93168F-8F82-4700-B411-D2EC8E6B1D9F}">
   <dimension ref="A1:G721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A708" workbookViewId="0">
-      <selection activeCell="C692" sqref="C692:C721"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G602" sqref="G602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,9 +5082,6 @@
       <c r="F212">
         <v>3</v>
       </c>
-      <c r="G212">
-        <v>-0.502</v>
-      </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
@@ -11216,7 +11213,7 @@
         <v>1</v>
       </c>
       <c r="G481">
-        <v>-2.1999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.25">
@@ -11880,7 +11877,7 @@
         <v>2</v>
       </c>
       <c r="G510">
-        <v>-2.1999999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.25">
@@ -11900,7 +11897,7 @@
         <v>2</v>
       </c>
       <c r="G511">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
@@ -13589,9 +13586,6 @@
       <c r="F585">
         <v>1</v>
       </c>
-      <c r="G585">
-        <v>-1.7000000000000001E-2</v>
-      </c>
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586">
@@ -13952,7 +13946,7 @@
         <v>1</v>
       </c>
       <c r="G601">
-        <v>-1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>